<commit_message>
Patch sector 2L emissions, assign to Industrial Sector
</commit_message>
<xml_diff>
--- a/data/national/ceds/data_aux/sector_mapping.xlsx
+++ b/data/national/ceds/data_aux/sector_mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FC66F7-0C90-4553-89DD-00CE60E58CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3BBEC1-4C49-4FD0-9E30-D6E190EEB904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sector_Mapping" sheetId="1" r:id="rId1"/>
@@ -2168,7 +2168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="1991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4799" uniqueCount="1991">
   <si>
     <t>CEDS_59</t>
   </si>
@@ -9302,6 +9302,86 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -10116,86 +10196,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -10214,41 +10214,41 @@
   <autoFilter ref="A1:AH199" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="IAMC" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CEDS_59" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CEDS_16" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CEDS_9" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="GAINS_SSP" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="GAINS_EMF30" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="SSP" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="IAMC" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CEDS_59" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CEDS_16" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CEDS_9" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="GAINS_SSP" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="GAINS_EMF30" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="SSP" dataDxfId="52"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="PRIMAP"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RCP"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EDGAR" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="EDGAR (IPCC Reference)" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Variables with an entry" dataDxfId="41"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Variables with an Entry in 9 Sectors or SSP" dataDxfId="40">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EDGAR" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="EDGAR (IPCC Reference)" dataDxfId="50"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Variables with an entry" dataDxfId="49"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Variables with an Entry in 9 Sectors or SSP" dataDxfId="48">
       <calculatedColumnFormula>IF(COUNTA(E2,H2)&gt;=1,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="CH4 Database" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CH4 Reporting" dataDxfId="38"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CO2 Database" dataDxfId="37"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="CO2 Reporting" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="N2O Database" dataDxfId="35"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="N2O Reporting" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BC Database" dataDxfId="33"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="BC Reporting" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CO Database" dataDxfId="31"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="CO Reporting" dataDxfId="30"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="NOx Database" dataDxfId="29"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="NOx Reporting" dataDxfId="28"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="OC Database" dataDxfId="27"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="OC Reporting" dataDxfId="26"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sulfur Database" dataDxfId="25"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Sulfur Reporting" dataDxfId="24"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="NH3 Database" dataDxfId="23"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="NH3 Reporting" dataDxfId="22"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="VOC Database" dataDxfId="21"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="VOC Reporting" dataDxfId="20"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="CH4 Database" dataDxfId="47"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CH4 Reporting" dataDxfId="46"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CO2 Database" dataDxfId="45"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="CO2 Reporting" dataDxfId="44"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="N2O Database" dataDxfId="43"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="N2O Reporting" dataDxfId="42"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BC Database" dataDxfId="41"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="BC Reporting" dataDxfId="40"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CO Database" dataDxfId="39"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="CO Reporting" dataDxfId="38"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="NOx Database" dataDxfId="37"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="NOx Reporting" dataDxfId="36"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="OC Database" dataDxfId="35"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="OC Reporting" dataDxfId="34"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sulfur Database" dataDxfId="33"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Sulfur Reporting" dataDxfId="32"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="NH3 Database" dataDxfId="31"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="NH3 Reporting" dataDxfId="30"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="VOC Database" dataDxfId="29"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="VOC Reporting" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10269,23 +10269,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table6" displayName="Table6" ref="A1:C98" totalsRowShown="0">
   <autoFilter ref="A1:C98" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable " dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Defintion" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable " dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Units" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Defintion" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="A2:E64" totalsRowShown="0" dataDxfId="15" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="A2:E64" totalsRowShown="0" dataDxfId="23" headerRowBorderDxfId="24">
   <autoFilter ref="A2:E64" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name=" EMF30_AGG" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Sector" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Fuel" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name=" EMF30_DET" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Description" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name=" EMF30_AGG" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Sector" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Fuel" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name=" EMF30_DET" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10318,25 +10318,25 @@
   <autoFilter ref="A1:M237" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Number"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="IAMC_high" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="IAMC_high" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="IAMC_low"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="CEDS_59" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="CEDS_16" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="CEDS_9" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="GAINS_SSP" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="GAINS_EMF30" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="SSP" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="CEDS_59" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="CEDS_16" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="CEDS_9" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="GAINS_SSP" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="GAINS_EMF30" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="SSP" dataDxfId="11"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="PRIMAP"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="RCP"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="EDGAR" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="EDGAR (IPCC Reference)" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="EDGAR" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="EDGAR (IPCC Reference)" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table7" displayName="Table7" ref="A1:C576" totalsRowShown="0" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table7" displayName="Table7" ref="A1:C576" totalsRowShown="0" tableBorderDxfId="8">
   <autoFilter ref="A1:C576" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Variable"/>
@@ -28282,42 +28282,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M95:M100 O95:AH103">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:AH4 O5:AH5 M6:AH8 M9 O9:AH9 M10:AH14 M15 O15:AH15 M16:AH23 M24 O24:AH24 M25:AH37 M38 O38:AH38 M39:AH64 M65 O65:AH65 M66:AH94 M103 M104:AH105 M106 O106:AH106 M107:AH118 M119:M120 O119:AH120 M121:AH137 M138 O138:AH138 M139:AH169 M170 O170:AH170 M171:AH198">
-    <cfRule type="cellIs" dxfId="57" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="56" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24">
-    <cfRule type="cellIs" dxfId="55" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38">
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N95:N103">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N106">
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N119:N120">
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38121,10 +38121,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B58F7F-6C03-4642-B26B-B1CECDED4318}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39571,16 +39571,19 @@
       <c r="A66" s="182"/>
       <c r="B66" s="183"/>
       <c r="C66" s="183"/>
-      <c r="D66" s="182" t="s">
-        <v>165</v>
+      <c r="F66" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="186"/>
       <c r="B67" s="188"/>
       <c r="C67" s="188"/>
-      <c r="D67" s="186" t="s">
-        <v>124</v>
+      <c r="D67" s="182" t="s">
+        <v>165</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
@@ -39590,8 +39593,8 @@
       <c r="A68" s="182"/>
       <c r="B68" s="183"/>
       <c r="C68" s="183"/>
-      <c r="D68" s="182" t="s">
-        <v>164</v>
+      <c r="D68" s="186" t="s">
+        <v>124</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
@@ -39601,12 +39604,17 @@
       <c r="A69" s="186"/>
       <c r="B69" s="188"/>
       <c r="C69" s="188"/>
-      <c r="D69" s="186" t="s">
-        <v>174</v>
+      <c r="D69" s="182" t="s">
+        <v>164</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D70" s="186" t="s">
+        <v>174</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F66" xr:uid="{88B58F7F-6C03-4642-B26B-B1CECDED4318}"/>
@@ -45697,26 +45705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f13b9d26-8c29-421b-be8e-d4ced6aabfd6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="40bf6408-2faa-4e3e-bfb6-796fd9260ca1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DD2EADC0C5A3441B70639C5993F2DD7" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="36f2c7b0485f7eef3a2cdf807850a570">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f13b9d26-8c29-421b-be8e-d4ced6aabfd6" xmlns:ns3="40bf6408-2faa-4e3e-bfb6-796fd9260ca1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4a2acc8113a45b187910e0089b2b296" ns2:_="" ns3:_="">
     <xsd:import namespace="f13b9d26-8c29-421b-be8e-d4ced6aabfd6"/>
@@ -45927,32 +45915,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91B8DBCD-77E3-4FB9-A215-A27AA03B4E59}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f13b9d26-8c29-421b-be8e-d4ced6aabfd6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40bf6408-2faa-4e3e-bfb6-796fd9260ca1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5596B5E-09CF-4256-BB1A-418B4FFC50C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f13b9d26-8c29-421b-be8e-d4ced6aabfd6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="40bf6408-2faa-4e3e-bfb6-796fd9260ca1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1474518-0351-4447-A117-D6A2A6667DC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45969,4 +45952,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5596B5E-09CF-4256-BB1A-418B4FFC50C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91B8DBCD-77E3-4FB9-A215-A27AA03B4E59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f13b9d26-8c29-421b-be8e-d4ced6aabfd6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40bf6408-2faa-4e3e-bfb6-796fd9260ca1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>